<commit_message>
Fixed truncation error in effluent data table
</commit_message>
<xml_diff>
--- a/ShinyApp/config.xlsx
+++ b/ShinyApp/config.xlsx
@@ -6,12 +6,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/colantonio_david_epa_gov/Documents/Profile/Desktop/11-1-23_IEX/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/burkhardt_jonathan_epa_gov/Documents/Profile/Desktop/Git/Water_Treatment_Models/ShinyApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="14_{8B255181-7898-4799-9A38-47AF8CA5F739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAF3C4A6-581F-413B-9DC2-94680B91E8A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90553765-B27D-4C23-95A1-91125137074D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>name</t>
   </si>
@@ -134,12 +134,6 @@
   </si>
   <si>
     <t>hours</t>
-  </si>
-  <si>
-    <t>conc</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -506,9 +500,9 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -530,7 +524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -541,7 +535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -552,7 +546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -563,7 +557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -574,7 +568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -585,7 +579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -596,7 +590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -604,7 +598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -615,7 +609,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -639,12 +633,12 @@
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -702,7 +696,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -731,7 +725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -760,7 +754,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -789,7 +783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -831,9 +825,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -853,7 +847,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -873,7 +867,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>40.5</v>
       </c>
@@ -901,34 +895,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3C450A-A43E-4263-8602-848D1B4D2897}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
+      <c r="B2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>